<commit_message>
Update Payment Section Trial Balance. 15-05-2019
</commit_message>
<xml_diff>
--- a/Data Files/PolicyData.xlsx
+++ b/Data Files/PolicyData.xlsx
@@ -71,10 +71,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -86,15 +86,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -111,6 +103,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -122,11 +122,49 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -138,13 +176,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -155,45 +186,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,6 +208,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -245,6 +245,72 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -269,43 +335,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,36 +365,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -365,6 +395,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -383,49 +419,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,39 +436,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -489,11 +456,59 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,21 +528,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -539,148 +539,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1035,7 +1035,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -1098,7 +1098,7 @@
         <v>14</v>
       </c>
       <c r="G2">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -1127,13 +1127,13 @@
         <v>15</v>
       </c>
       <c r="G3">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Policy Creating/Account Matching/Trial Balance . Completed
</commit_message>
<xml_diff>
--- a/Data Files/PolicyData.xlsx
+++ b/Data Files/PolicyData.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="24000" windowHeight="10485" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="20310" windowHeight="8325" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="PolicyData" sheetId="1" r:id="rId1"/>
+    <sheet name="Commission" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
   <si>
     <t>AlertOption</t>
   </si>
@@ -66,6 +66,15 @@
     <t>StandAlone</t>
   </si>
   <si>
+    <t>Duplex</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>FirmHouse</t>
+  </si>
+  <si>
     <t>PolicyNo</t>
   </si>
   <si>
@@ -78,16 +87,157 @@
     <t>BrokerComission</t>
   </si>
   <si>
-    <t>DASD/POLICY/003187</t>
-  </si>
-  <si>
-    <t>DASD/POLICY/003189</t>
+    <t>LondonBrokerComm</t>
+  </si>
+  <si>
+    <t>TotalPremium</t>
+  </si>
+  <si>
+    <t>DASD/POLICY/003277</t>
+  </si>
+  <si>
+    <t>USD 330.00</t>
+  </si>
+  <si>
+    <t>DASD/POLICY/003279</t>
+  </si>
+  <si>
+    <t>USD 660.00</t>
+  </si>
+  <si>
+    <t>DASD/POLICY/003281</t>
+  </si>
+  <si>
+    <t>USD 770.00</t>
+  </si>
+  <si>
+    <t>DASD/POLICY/003283</t>
+  </si>
+  <si>
+    <t>DASD/POLICY/003285</t>
+  </si>
+  <si>
+    <t>USD 297.00</t>
+  </si>
+  <si>
+    <t>DASD/POLICY/003287</t>
+  </si>
+  <si>
+    <t>USD 374.00</t>
+  </si>
+  <si>
+    <t>DASD/POLICY/003289</t>
+  </si>
+  <si>
+    <t>USD 616.00</t>
+  </si>
+  <si>
+    <t>DASD/POLICY/003291</t>
+  </si>
+  <si>
+    <t>DASD/POLICY/003293</t>
+  </si>
+  <si>
+    <t>USD 385.00</t>
+  </si>
+  <si>
+    <t>DASD/POLICY/003295</t>
+  </si>
+  <si>
+    <t>USD 638.00</t>
   </si>
   <si>
     <t>145.50</t>
   </si>
   <si>
     <t>291.00</t>
+  </si>
+  <si>
+    <t>339.50</t>
+  </si>
+  <si>
+    <t>130.95</t>
+  </si>
+  <si>
+    <t>164.90</t>
+  </si>
+  <si>
+    <t>271.60</t>
+  </si>
+  <si>
+    <t>169.75</t>
+  </si>
+  <si>
+    <t>281.30</t>
+  </si>
+  <si>
+    <t>90.00</t>
+  </si>
+  <si>
+    <t>180.00</t>
+  </si>
+  <si>
+    <t>210.00</t>
+  </si>
+  <si>
+    <t>81.00</t>
+  </si>
+  <si>
+    <t>102.00</t>
+  </si>
+  <si>
+    <t>168.00</t>
+  </si>
+  <si>
+    <t>105.00</t>
+  </si>
+  <si>
+    <t>174.00</t>
+  </si>
+  <si>
+    <t>84.00</t>
+  </si>
+  <si>
+    <t>196.00</t>
+  </si>
+  <si>
+    <t>75.60</t>
+  </si>
+  <si>
+    <t>95.20</t>
+  </si>
+  <si>
+    <t>156.80</t>
+  </si>
+  <si>
+    <t>98.00</t>
+  </si>
+  <si>
+    <t>162.40</t>
+  </si>
+  <si>
+    <t>10.50</t>
+  </si>
+  <si>
+    <t>21.00</t>
+  </si>
+  <si>
+    <t>24.50</t>
+  </si>
+  <si>
+    <t>9.45</t>
+  </si>
+  <si>
+    <t>11.90</t>
+  </si>
+  <si>
+    <t>19.60</t>
+  </si>
+  <si>
+    <t>12.25</t>
+  </si>
+  <si>
+    <t>20.30</t>
   </si>
 </sst>
 </file>
@@ -95,12 +245,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -114,15 +264,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -180,13 +336,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +360,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -279,6 +435,84 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -291,175 +525,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,142 +731,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -719,6 +875,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1039,19 +1198,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A2:$XFD2 A1"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="18.5809523809524" collapsed="true"/>
     <col min="2" max="3" customWidth="true" width="9.14285714285714" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="16.8571428571429" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="6" max="1025" customWidth="true" width="9.14285714285714" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="8.71428571428571" collapsed="true"/>
+    <col min="7" max="1025" customWidth="true" width="9.14285714285714" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.5" spans="1:9">
@@ -1139,6 +1299,238 @@
       </c>
       <c r="I3" s="2">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="4" ht="25.5" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>4000</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" ht="25.5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>5000</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" ht="25.5" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>1500</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="7" ht="25.5" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>1400</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" ht="25.5" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>4100</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9" ht="25.5" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>3000</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" ht="25.5" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10">
+        <v>2500</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" ht="25.5" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>800</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
@@ -1151,49 +1543,241 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.0285714285714" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="21.5714285714286" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="15.7142857142857" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.8571428571429" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.7142857142857" collapsed="true"/>
-    <col min="5" max="1025" customWidth="true" width="9.14285714285714" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.1428571428571" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.1428571428571" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.4285714285714" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7142857142857" collapsed="true"/>
+    <col min="7" max="1026" customWidth="true" width="9.14285714285714" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14" customHeight="1" spans="1:4">
+    <row r="1" ht="14" customHeight="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>